<commit_message>
données excell test + modifs dataframe dans mail.py
</commit_message>
<xml_diff>
--- a/Excel_type.xlsx
+++ b/Excel_type.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="60">
   <si>
     <t>GlobalID</t>
   </si>
@@ -179,6 +179,21 @@
   </si>
   <si>
     <t>60222876-f542-4b59-a34d-e2ecc13c45d6</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arborial </t>
+  </si>
+  <si>
+    <t>VNF Musee</t>
+  </si>
+  <si>
+    <t>Rue barbes</t>
+  </si>
+  <si>
+    <t>60222876-f542-4b59-a34d-e2ecc13c45d7</t>
   </si>
 </sst>
 </file>
@@ -525,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -536,19 +551,19 @@
     <col min="1" max="1" width="8.77734375" style="1"/>
     <col min="2" max="2" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="52.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.5546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="24.21875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.88671875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="18.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="8.77734375" style="1"/>
+    <col min="4" max="5" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="52.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.5546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="24.21875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.88671875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,40 +574,43 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -602,541 +620,606 @@
       <c r="C2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <v>44006.416666666701</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <v>44280.458333333299</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <v>44097.416666666701</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <v>44280.458333333299</v>
       </c>
-      <c r="M2" s="1">
+      <c r="N2" s="1">
         <v>1.4508715065584601</v>
       </c>
-      <c r="N2" s="1">
+      <c r="O2" s="1">
         <v>43.613362333711798</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>-1</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>44028.416666666701</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <v>44119.416666666701</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="2">
+      <c r="K3" s="2">
         <v>44119.416666666701</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" s="1">
+      <c r="L3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" s="1">
         <v>-0.606940042488475</v>
       </c>
-      <c r="N3" s="1">
+      <c r="O3" s="1">
         <v>44.785392971202</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>1</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>44148.458333333299</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <v>44787.416666666701</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="2">
+      <c r="K4" s="2">
         <v>44787.416666666701</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="2">
+      <c r="M4" s="2">
         <v>44787.416666666701</v>
       </c>
-      <c r="M4" s="1">
+      <c r="N4" s="1">
         <v>1.3586176679861801</v>
       </c>
-      <c r="N4" s="1">
+      <c r="O4" s="1">
         <v>43.575781061781697</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>44148.458333333299</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M5" s="1">
+      <c r="L5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" s="1">
         <v>3.733641</v>
       </c>
-      <c r="N5" s="1">
+      <c r="O5" s="1">
         <v>43.794552500000002</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="1">
         <v>1</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>44161.458333333299</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <v>45165.416666666701</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="2">
+      <c r="K6" s="2">
         <v>44435.416666666701</v>
       </c>
-      <c r="M6" s="1">
+      <c r="N6" s="1">
         <v>4.61510608498455</v>
       </c>
-      <c r="N6" s="1">
+      <c r="O6" s="1">
         <v>43.672028374676998</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="1">
         <v>2</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>44161.458333333299</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="2">
+      <c r="I7" s="2">
         <v>45165.416666666701</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M7" s="1">
+      <c r="J7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N7" s="1">
         <v>4.6150316083691303</v>
       </c>
-      <c r="N7" s="1">
+      <c r="O7" s="1">
         <v>43.671951125470798</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="1">
         <v>3</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>44161.458333333299</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I8" s="2">
         <v>44252.458333333299</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J8" s="2">
+      <c r="K8" s="2">
         <v>44435.416666666701</v>
       </c>
-      <c r="M8" s="1">
+      <c r="N8" s="1">
         <v>4.6149481518303004</v>
       </c>
-      <c r="N8" s="1">
+      <c r="O8" s="1">
         <v>43.671876063027398</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>1</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>44162.458333333299</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M9" s="1">
+      <c r="J9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N9" s="1">
         <v>2.3615329293793899</v>
       </c>
-      <c r="N9" s="1">
+      <c r="O9" s="1">
         <v>43.229760237390799</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:15">
       <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>2</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <v>44162.458333333299</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H10" s="2">
+      <c r="I10" s="2">
         <v>44436.416666666701</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M10" s="1">
+      <c r="J10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" s="1">
         <v>2.36169609823625</v>
       </c>
-      <c r="N10" s="1">
+      <c r="O10" s="1">
         <v>43.229861789738401</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:15">
       <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>3</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>44162.458333333299</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="2">
+      <c r="I11" s="2">
         <v>44436.416666666701</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M11" s="1">
+      <c r="J11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N11" s="1">
         <v>2.3614266477594299</v>
       </c>
-      <c r="N11" s="1">
+      <c r="O11" s="1">
         <v>43.2296460283507</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:15">
       <c r="A12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>4</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <v>44162.458333333299</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="2">
+      <c r="I12" s="2">
         <v>45166.416666666701</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M12" s="1">
+      <c r="J12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N12" s="1">
         <v>2.3622165583285599</v>
       </c>
-      <c r="N12" s="1">
+      <c r="O12" s="1">
         <v>43.229638211172002</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:15">
       <c r="A13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <v>5</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F13" s="2">
         <v>44162.458333333299</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="2">
+      <c r="I13" s="2">
         <v>45166.416666666701</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M13" s="1">
+      <c r="J13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N13" s="1">
         <v>2.3616839609967699</v>
       </c>
-      <c r="N13" s="1">
+      <c r="O13" s="1">
         <v>43.229857646599697</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:15">
       <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="1">
         <v>1</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F14" s="2">
         <v>44161.458333333299</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I14" s="2">
         <v>44800.416666666701</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M14" s="1">
+      <c r="J14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N14" s="1">
         <v>3.7336041999999998</v>
       </c>
-      <c r="N14" s="1">
+      <c r="O14" s="1">
         <v>43.794758399999999</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="1">
         <v>2</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F15" s="2">
         <v>44161.458333333299</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H15" s="2">
+      <c r="I15" s="2">
         <v>44800.416666666701</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M15" s="1">
+      <c r="J15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N15" s="1">
         <v>3.7336041999999998</v>
       </c>
-      <c r="N15" s="1">
+      <c r="O15" s="1">
         <v>43.794758399999999</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:15">
       <c r="A16" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="1">
         <v>3</v>
       </c>
-      <c r="E16" s="2">
+      <c r="F16" s="2">
         <v>44161.458333333299</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="2">
+      <c r="I16" s="2">
         <v>44800.416666666701</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M16" s="1">
+      <c r="J16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N16" s="1">
         <v>3.7336041999999998</v>
       </c>
-      <c r="N16" s="1">
+      <c r="O16" s="1">
         <v>43.794758399999999</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:15">
       <c r="A17" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="1">
         <v>5</v>
       </c>
-      <c r="E17" s="2">
-        <v>44161.458333333299</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="2">
+        <v>44151.458333333336</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H17" s="2">
-        <v>44800.416666666701</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M17" s="1">
+      <c r="I17" s="2">
+        <v>44151.458333333336</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N17" s="1">
         <v>3.7336041999999998</v>
       </c>
-      <c r="N17" s="1">
+      <c r="O17" s="1">
+        <v>43.794758399999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="1">
+        <v>10</v>
+      </c>
+      <c r="F18" s="2">
+        <v>44142.458333333336</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" s="2">
+        <v>44142.458333333336</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M18" s="2">
+        <v>44216.458333333336</v>
+      </c>
+      <c r="N18" s="1">
+        <v>3.7336041999999998</v>
+      </c>
+      <c r="O18" s="1">
         <v>43.794758399999999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
retrait fichiers inutiles + finalisation mail + logo + modifs test excel
</commit_message>
<xml_diff>
--- a/Excel_type.xlsx
+++ b/Excel_type.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="63">
   <si>
     <t>GlobalID</t>
   </si>
@@ -194,6 +194,15 @@
   </si>
   <si>
     <t>60222876-f542-4b59-a34d-e2ecc13c45d7</t>
+  </si>
+  <si>
+    <t>60222876-f542-4b59-a34d-e2ecc13c45d9</t>
+  </si>
+  <si>
+    <t>quochiepdao92@gmail.com</t>
+  </si>
+  <si>
+    <t>lothesven@yahoo.fr</t>
   </si>
 </sst>
 </file>
@@ -540,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -1151,6 +1160,9 @@
       <c r="B17" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="C17" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="D17" s="1" t="s">
         <v>58</v>
       </c>
@@ -1189,6 +1201,9 @@
       <c r="B18" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="C18" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="D18" s="1" t="s">
         <v>57</v>
       </c>
@@ -1223,8 +1238,54 @@
         <v>43.794758399999999</v>
       </c>
     </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="1">
+        <v>5</v>
+      </c>
+      <c r="F19" s="2">
+        <v>44151.458333333336</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="2">
+        <v>44151.458333333336</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N19" s="1">
+        <v>3.7336041999999998</v>
+      </c>
+      <c r="O19" s="1">
+        <v>43.794758399999999</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C17" r:id="rId1"/>
+    <hyperlink ref="C19" r:id="rId2"/>
+    <hyperlink ref="C18" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>